<commit_message>
Criado novas validações em Conferencia Bancaria
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação de Taxas.xlsx
+++ b/cypress/downloads/Conciliação de Taxas.xlsx
@@ -262,20 +262,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="20.71" min="1" max="1" customWidth="1"/>
-    <col width="18.14" min="2" max="2" customWidth="1"/>
-    <col width="15.57" min="3" max="3" customWidth="1"/>
-    <col width="17.86" min="4" max="4" customWidth="1"/>
-    <col width="16.14" min="5" max="5" customWidth="1"/>
+    <col width="20.57" min="1" max="1" customWidth="1"/>
+    <col width="17.86" min="2" max="2" customWidth="1"/>
+    <col width="15.43" min="3" max="3" customWidth="1"/>
+    <col width="17.71" min="4" max="4" customWidth="1"/>
+    <col width="16" min="5" max="5" customWidth="1"/>
     <col width="10.29" min="6" max="6" customWidth="1"/>
-    <col width="20.43" min="7" max="7" customWidth="1"/>
-    <col width="13.57" min="8" max="8" customWidth="1"/>
-    <col width="17" min="9" max="9" customWidth="1"/>
-    <col width="21.14" min="10" max="10" customWidth="1"/>
-    <col width="18.86" min="11" max="11" customWidth="1"/>
-    <col width="21.86" min="12" max="12" customWidth="1"/>
-    <col width="26" min="13" max="13" customWidth="1"/>
-    <col width="12.29" min="14" max="14" customWidth="1"/>
+    <col width="20.14" min="7" max="7" customWidth="1"/>
+    <col width="13.43" min="8" max="8" customWidth="1"/>
+    <col width="16.86" min="9" max="9" customWidth="1"/>
+    <col width="21" min="10" max="10" customWidth="1"/>
+    <col width="18.71" min="11" max="11" customWidth="1"/>
+    <col width="21.57" min="12" max="12" customWidth="1"/>
+    <col width="25.71" min="13" max="13" customWidth="1"/>
+    <col width="12.14" min="14" max="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Criado validações novas em todas as telas
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação de Taxas.xlsx
+++ b/cypress/downloads/Conciliação de Taxas.xlsx
@@ -59,106 +59,106 @@
     <t>Qtde.</t>
   </si>
   <si>
+    <t>000000080683215</t>
+  </si>
+  <si>
+    <t>000000012784869</t>
+  </si>
+  <si>
+    <t>82123891000138</t>
+  </si>
+  <si>
+    <t>EMPRESA MODELO</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>Ticket Flex</t>
+  </si>
+  <si>
+    <t>000000008781044</t>
+  </si>
+  <si>
+    <t>TICKET ALIMENTACAO</t>
+  </si>
+  <si>
+    <t>000000080683312</t>
+  </si>
+  <si>
+    <t>000000008784337</t>
+  </si>
+  <si>
+    <t>033090890000129</t>
+  </si>
+  <si>
+    <t>Sodexo</t>
+  </si>
+  <si>
+    <t>SODEXO REFEICAO</t>
+  </si>
+  <si>
+    <t>Comprocard</t>
+  </si>
+  <si>
+    <t>Comprocard Crédito</t>
+  </si>
+  <si>
+    <t>000000008784329</t>
+  </si>
+  <si>
+    <t>TICKET REFEICAO</t>
+  </si>
+  <si>
+    <t>000000007815071</t>
+  </si>
+  <si>
+    <t>000000007815066</t>
+  </si>
+  <si>
+    <t>UpBrasil</t>
+  </si>
+  <si>
+    <t>UpBrasil Convênio</t>
+  </si>
+  <si>
     <t>013998257000126</t>
   </si>
   <si>
-    <t>82123891000138</t>
-  </si>
-  <si>
-    <t>EMPRESA MODELO</t>
-  </si>
-  <si>
     <t>Valecard</t>
   </si>
   <si>
     <t>Valecard Voucher</t>
   </si>
   <si>
+    <t>000000001438301</t>
+  </si>
+  <si>
+    <t>000000000143830</t>
+  </si>
+  <si>
+    <t>Green Card</t>
+  </si>
+  <si>
+    <t>Green Card Débito</t>
+  </si>
+  <si>
+    <t>000000008781052</t>
+  </si>
+  <si>
     <t>033091040000145</t>
   </si>
   <si>
+    <t>Cabal</t>
+  </si>
+  <si>
+    <t>CABAL VOUCHER</t>
+  </si>
+  <si>
     <t>VR</t>
   </si>
   <si>
     <t>VR REFEICAO</t>
-  </si>
-  <si>
-    <t>Sodexo</t>
-  </si>
-  <si>
-    <t>SODEXO REFEICAO</t>
-  </si>
-  <si>
-    <t>033090890000129</t>
-  </si>
-  <si>
-    <t>000000080683312</t>
-  </si>
-  <si>
-    <t>000000008784337</t>
-  </si>
-  <si>
-    <t>Ticket</t>
-  </si>
-  <si>
-    <t>TICKET ALIMENTACAO</t>
-  </si>
-  <si>
-    <t>000000008784329</t>
-  </si>
-  <si>
-    <t>TICKET REFEICAO</t>
-  </si>
-  <si>
-    <t>000000080683215</t>
-  </si>
-  <si>
-    <t>000000008781044</t>
-  </si>
-  <si>
-    <t>000000008781052</t>
-  </si>
-  <si>
-    <t>Cabal</t>
-  </si>
-  <si>
-    <t>CABAL VOUCHER</t>
-  </si>
-  <si>
-    <t>000000007815066</t>
-  </si>
-  <si>
-    <t>UpBrasil</t>
-  </si>
-  <si>
-    <t>UpBrasil Convênio</t>
-  </si>
-  <si>
-    <t>000000007815071</t>
-  </si>
-  <si>
-    <t>000000012784869</t>
-  </si>
-  <si>
-    <t>Ticket Flex</t>
-  </si>
-  <si>
-    <t>000000001438301</t>
-  </si>
-  <si>
-    <t>000000000143830</t>
-  </si>
-  <si>
-    <t>Green Card</t>
-  </si>
-  <si>
-    <t>Green Card Débito</t>
-  </si>
-  <si>
-    <t>Comprocard</t>
-  </si>
-  <si>
-    <t>Comprocard Crédito</t>
   </si>
   <si>
     <t>127.811,42</t>
@@ -263,7 +263,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col width="20.57" min="1" max="1" customWidth="1"/>
-    <col width="17.86" min="2" max="2" customWidth="1"/>
+    <col width="18" min="2" max="2" customWidth="1"/>
     <col width="15.43" min="3" max="3" customWidth="1"/>
     <col width="17.71" min="4" max="4" customWidth="1"/>
     <col width="16" min="5" max="5" customWidth="1"/>
@@ -326,39 +326,41 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s"/>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>3.71</v>
+        <v>6.57</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>2.7</v>
+        <v>5.94</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>0.3</v>
+        <v>5.94</v>
       </c>
       <c r="M2" s="6" t="n">
-        <v>0.01</v>
+        <v>0.39</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>1</v>
@@ -368,165 +370,171 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s"/>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>164.29</v>
+        <v>62.05</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>2.79</v>
+        <v>6.01</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>0.39</v>
+        <v>6.01</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>0.64</v>
+        <v>3.73</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s"/>
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>118422.66</v>
+        <v>29.75</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>2.8</v>
+        <v>5.98</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>0.4</v>
+        <v>5.98</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>473.69</v>
+        <v>1.78</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s"/>
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>133.63</v>
+        <v>15.52</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>2.81</v>
+        <v>6.89</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>0.41</v>
+        <v>6.89</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>0.55</v>
+        <v>1.07</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s"/>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v>9.99</v>
+        <v>4.79</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>6.81</v>
+        <v>5.85</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>6.81</v>
+        <v>5.85</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>0.68</v>
+        <v>0.28</v>
       </c>
       <c r="N6" s="5" t="n">
         <v>1</v>
@@ -534,17 +542,19 @@
     </row>
     <row r="7" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>45170</v>
@@ -556,63 +566,63 @@
         <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v>282</v>
+        <v>299.89</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>6.85</v>
+        <v>6</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>6.85</v>
+        <v>6</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>19.32</v>
+        <v>17.99</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>0.01</v>
+        <v>5.79</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>0</v>
+        <v>6.04</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>0</v>
+        <v>6.04</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="N8" s="5" t="n">
         <v>1</v>
@@ -620,43 +630,43 @@
     </row>
     <row r="9" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>69.44</v>
+        <v>150</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>4.79</v>
+        <v>9</v>
       </c>
       <c r="N9" s="5" t="n">
         <v>1</v>
@@ -664,43 +674,43 @@
     </row>
     <row r="10" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>15.52</v>
+        <v>31.95</v>
       </c>
       <c r="J10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>6.89</v>
+        <v>5.01</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>6.89</v>
+        <v>5.01</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>1.07</v>
+        <v>1.6</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>1</v>
@@ -708,60 +718,56 @@
     </row>
     <row r="11" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s"/>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="6" t="n">
-        <v>6.22</v>
+        <v>164.29</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>5.95</v>
+        <v>2.79</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>5.95</v>
+        <v>0.39</v>
       </c>
       <c r="M11" s="6" t="n">
-        <v>0.37</v>
+        <v>0.64</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s"/>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>27</v>
@@ -776,19 +782,19 @@
         <v>0</v>
       </c>
       <c r="I12" s="6" t="n">
-        <v>29.75</v>
+        <v>9.59</v>
       </c>
       <c r="J12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>5.98</v>
+        <v>5.94</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>5.98</v>
+        <v>5.94</v>
       </c>
       <c r="M12" s="6" t="n">
-        <v>1.78</v>
+        <v>0.57</v>
       </c>
       <c r="N12" s="5" t="n">
         <v>1</v>
@@ -796,192 +802,190 @@
     </row>
     <row r="13" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="6" t="n">
-        <v>174.71</v>
+        <v>145.29</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>5.99</v>
+        <v>6.8</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>5.99</v>
+        <v>6.8</v>
       </c>
       <c r="M13" s="6" t="n">
-        <v>10.47</v>
+        <v>9.88</v>
       </c>
       <c r="N13" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="6" t="n">
-        <v>1136</v>
+        <v>58.01</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>6</v>
+        <v>7.38</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>6</v>
+        <v>7.38</v>
       </c>
       <c r="M14" s="6" t="n">
-        <v>68.16</v>
+        <v>4.28</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="6" t="n">
-        <v>104.65</v>
+        <v>266.69</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>6.01</v>
+        <v>5.99</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>6.01</v>
+        <v>5.99</v>
       </c>
       <c r="M15" s="6" t="n">
-        <v>6.29</v>
+        <v>15.97</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="6" t="n">
-        <v>33.9</v>
+        <v>490.6</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="5" t="n">
-        <v>6.02</v>
+        <v>6</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>6.02</v>
+        <v>6</v>
       </c>
       <c r="M16" s="6" t="n">
-        <v>2.04</v>
+        <v>29.44</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s"/>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>27</v>
@@ -996,19 +1000,19 @@
         <v>0</v>
       </c>
       <c r="I17" s="6" t="n">
-        <v>5.79</v>
+        <v>12.71</v>
       </c>
       <c r="J17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>6.04</v>
+        <v>5.9</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>6.04</v>
+        <v>5.9</v>
       </c>
       <c r="M17" s="6" t="n">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="N17" s="5" t="n">
         <v>1</v>
@@ -1016,163 +1020,163 @@
     </row>
     <row r="18" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="6" t="n">
-        <v>0.99</v>
+        <v>174.71</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>6.06</v>
+        <v>5.99</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>6.06</v>
+        <v>5.99</v>
       </c>
       <c r="M18" s="6" t="n">
-        <v>0.06</v>
+        <v>10.47</v>
       </c>
       <c r="N18" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="6" t="n">
-        <v>0.02</v>
+        <v>51.86</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>0</v>
+        <v>6.02</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>0</v>
+        <v>6.02</v>
       </c>
       <c r="M19" s="6" t="n">
-        <v>0</v>
+        <v>3.12</v>
       </c>
       <c r="N19" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="6" t="n">
-        <v>150</v>
+        <v>62.32</v>
       </c>
       <c r="J20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K20" s="5" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="M20" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="N20" s="5" t="n">
         <v>6</v>
-      </c>
-      <c r="L20" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="M20" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="N20" s="5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="6" t="n">
-        <v>40.42</v>
+        <v>152.11</v>
       </c>
       <c r="J21" s="5" t="n">
         <v>0</v>
@@ -1184,24 +1188,22 @@
         <v>6.01</v>
       </c>
       <c r="M21" s="6" t="n">
-        <v>2.43</v>
+        <v>9.14</v>
       </c>
       <c r="N21" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s"/>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>27</v>
@@ -1216,36 +1218,34 @@
         <v>0</v>
       </c>
       <c r="I22" s="6" t="n">
-        <v>9.19</v>
+        <v>75.74</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>5.98</v>
+        <v>7.91</v>
       </c>
       <c r="L22" s="5" t="n">
-        <v>5.98</v>
+        <v>7.91</v>
       </c>
       <c r="M22" s="6" t="n">
-        <v>0.55</v>
+        <v>5.99</v>
       </c>
       <c r="N22" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s"/>
       <c r="C23" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>27</v>
@@ -1260,195 +1260,195 @@
         <v>0</v>
       </c>
       <c r="I23" s="6" t="n">
-        <v>121.15</v>
+        <v>25.47</v>
       </c>
       <c r="J23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>5.99</v>
+        <v>5.89</v>
       </c>
       <c r="L23" s="5" t="n">
-        <v>5.99</v>
+        <v>5.89</v>
       </c>
       <c r="M23" s="6" t="n">
-        <v>7.26</v>
+        <v>1.5</v>
       </c>
       <c r="N23" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="6" t="n">
-        <v>299.89</v>
+        <v>6.08</v>
       </c>
       <c r="J24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K24" s="5" t="n">
-        <v>6</v>
+        <v>5.92</v>
       </c>
       <c r="L24" s="5" t="n">
-        <v>6</v>
+        <v>5.92</v>
       </c>
       <c r="M24" s="6" t="n">
-        <v>17.99</v>
+        <v>0.36</v>
       </c>
       <c r="N24" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="6" t="n">
-        <v>62.05</v>
+        <v>20.25</v>
       </c>
       <c r="J25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K25" s="5" t="n">
-        <v>6.01</v>
+        <v>5.98</v>
       </c>
       <c r="L25" s="5" t="n">
-        <v>6.01</v>
+        <v>5.98</v>
       </c>
       <c r="M25" s="6" t="n">
-        <v>3.73</v>
+        <v>1.21</v>
       </c>
       <c r="N25" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="6" t="n">
-        <v>51.86</v>
+        <v>40.29</v>
       </c>
       <c r="J26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K26" s="5" t="n">
-        <v>6.02</v>
+        <v>6.03</v>
       </c>
       <c r="L26" s="5" t="n">
-        <v>6.02</v>
+        <v>6.03</v>
       </c>
       <c r="M26" s="6" t="n">
-        <v>3.12</v>
+        <v>2.43</v>
       </c>
       <c r="N26" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="6" t="n">
-        <v>6.08</v>
+        <v>9.19</v>
       </c>
       <c r="J27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K27" s="5" t="n">
-        <v>5.92</v>
+        <v>5.98</v>
       </c>
       <c r="L27" s="5" t="n">
-        <v>5.92</v>
+        <v>5.98</v>
       </c>
       <c r="M27" s="6" t="n">
-        <v>0.36</v>
+        <v>0.55</v>
       </c>
       <c r="N27" s="5" t="n">
         <v>1</v>
@@ -1456,63 +1456,61 @@
     </row>
     <row r="28" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B28" s="3" t="s"/>
       <c r="C28" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F28" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H28" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="6" t="n">
-        <v>490.6</v>
+        <v>133.63</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K28" s="5" t="n">
-        <v>6</v>
+        <v>2.81</v>
       </c>
       <c r="L28" s="5" t="n">
-        <v>6</v>
+        <v>0.41</v>
       </c>
       <c r="M28" s="6" t="n">
-        <v>29.44</v>
+        <v>0.55</v>
       </c>
       <c r="N28" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>45170</v>
@@ -1524,19 +1522,19 @@
         <v>0</v>
       </c>
       <c r="I29" s="6" t="n">
-        <v>73.57</v>
+        <v>0.02</v>
       </c>
       <c r="J29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="5" t="n">
-        <v>6.01</v>
+        <v>0</v>
       </c>
       <c r="L29" s="5" t="n">
-        <v>6.01</v>
+        <v>0</v>
       </c>
       <c r="M29" s="6" t="n">
-        <v>4.42</v>
+        <v>0</v>
       </c>
       <c r="N29" s="5" t="n">
         <v>2</v>
@@ -1544,83 +1542,85 @@
     </row>
     <row r="30" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="3" t="s"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="H30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="6" t="n">
-        <v>4.98</v>
+        <v>104.65</v>
       </c>
       <c r="J30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K30" s="5" t="n">
-        <v>5.02</v>
+        <v>6.01</v>
       </c>
       <c r="L30" s="5" t="n">
-        <v>5.02</v>
+        <v>6.01</v>
       </c>
       <c r="M30" s="6" t="n">
-        <v>0.25</v>
+        <v>6.29</v>
       </c>
       <c r="N30" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s"/>
       <c r="C31" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="6" t="n">
-        <v>1.19</v>
+        <v>2.49</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K31" s="5" t="n">
-        <v>5.04</v>
+        <v>8.03</v>
       </c>
       <c r="L31" s="5" t="n">
-        <v>5.04</v>
+        <v>8.03</v>
       </c>
       <c r="M31" s="6" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="N31" s="5" t="n">
         <v>1</v>
@@ -1628,44 +1628,46 @@
     </row>
     <row r="32" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="3" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="6" t="n">
-        <v>31.15</v>
+        <v>37.18</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="5" t="n">
-        <v>6.48</v>
+        <v>5.97</v>
       </c>
       <c r="L32" s="5" t="n">
-        <v>6.48</v>
+        <v>5.97</v>
       </c>
       <c r="M32" s="6" t="n">
-        <v>2.02</v>
+        <v>2.22</v>
       </c>
       <c r="N32" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -1674,37 +1676,37 @@
       </c>
       <c r="B33" s="3" t="s"/>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I33" s="6" t="n">
-        <v>82.34</v>
+        <v>39.65</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="5" t="n">
-        <v>6.5</v>
+        <v>6.51</v>
       </c>
       <c r="L33" s="5" t="n">
-        <v>6.5</v>
+        <v>6.51</v>
       </c>
       <c r="M33" s="6" t="n">
-        <v>5.35</v>
+        <v>2.58</v>
       </c>
       <c r="N33" s="5" t="n">
         <v>1</v>
@@ -1716,37 +1718,37 @@
       </c>
       <c r="B34" s="3" t="s"/>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="n">
-        <v>39.65</v>
+        <v>4.98</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="5" t="n">
-        <v>6.51</v>
+        <v>5.02</v>
       </c>
       <c r="L34" s="5" t="n">
-        <v>6.51</v>
+        <v>5.02</v>
       </c>
       <c r="M34" s="6" t="n">
-        <v>2.58</v>
+        <v>0.25</v>
       </c>
       <c r="N34" s="5" t="n">
         <v>1</v>
@@ -1754,87 +1756,83 @@
     </row>
     <row r="35" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3" t="s"/>
+      <c r="C35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="H35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="n">
-        <v>10.99</v>
+        <v>118422.66</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K35" s="5" t="n">
-        <v>7.37</v>
+        <v>2.8</v>
       </c>
       <c r="L35" s="5" t="n">
-        <v>7.37</v>
+        <v>0.4</v>
       </c>
       <c r="M35" s="6" t="n">
-        <v>0.81</v>
+        <v>473.69</v>
       </c>
       <c r="N35" s="5" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B36" s="3" t="s"/>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I36" s="6" t="n">
-        <v>58.01</v>
+        <v>42.58</v>
       </c>
       <c r="J36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K36" s="5" t="n">
-        <v>7.38</v>
+        <v>7.89</v>
       </c>
       <c r="L36" s="5" t="n">
-        <v>7.38</v>
+        <v>7.89</v>
       </c>
       <c r="M36" s="6" t="n">
-        <v>4.28</v>
+        <v>3.36</v>
       </c>
       <c r="N36" s="5" t="n">
         <v>2</v>
@@ -1842,87 +1840,85 @@
     </row>
     <row r="37" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B37" s="3" t="s"/>
       <c r="C37" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F37" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I37" s="6" t="n">
-        <v>172.07</v>
+        <v>33</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K37" s="5" t="n">
-        <v>7.39</v>
+        <v>5.91</v>
       </c>
       <c r="L37" s="5" t="n">
-        <v>7.39</v>
+        <v>5.91</v>
       </c>
       <c r="M37" s="6" t="n">
-        <v>12.72</v>
+        <v>1.95</v>
       </c>
       <c r="N37" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F38" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I38" s="6" t="n">
-        <v>28.92</v>
+        <v>22.1</v>
       </c>
       <c r="J38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K38" s="5" t="n">
-        <v>7.4</v>
+        <v>5.02</v>
       </c>
       <c r="L38" s="5" t="n">
-        <v>7.4</v>
+        <v>5.02</v>
       </c>
       <c r="M38" s="6" t="n">
-        <v>2.14</v>
+        <v>1.11</v>
       </c>
       <c r="N38" s="5" t="n">
         <v>1</v>
@@ -1930,87 +1926,83 @@
     </row>
     <row r="39" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B39" s="3" t="s"/>
       <c r="C39" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I39" s="6" t="n">
-        <v>68.38</v>
+        <v>19.56</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>9.07</v>
+        <v>7.92</v>
       </c>
       <c r="L39" s="5" t="n">
-        <v>9.07</v>
+        <v>7.92</v>
       </c>
       <c r="M39" s="6" t="n">
-        <v>6.2</v>
+        <v>1.55</v>
       </c>
       <c r="N39" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B40" s="3" t="s"/>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="6" t="n">
-        <v>42.24</v>
+        <v>31.15</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K40" s="5" t="n">
-        <v>5</v>
+        <v>6.48</v>
       </c>
       <c r="L40" s="5" t="n">
-        <v>5</v>
+        <v>6.48</v>
       </c>
       <c r="M40" s="6" t="n">
-        <v>2.11</v>
+        <v>2.02</v>
       </c>
       <c r="N40" s="5" t="n">
         <v>1</v>
@@ -2018,104 +2010,102 @@
     </row>
     <row r="41" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F41" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="6" t="n">
-        <v>31.95</v>
+        <v>2137.12</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>5.01</v>
+        <v>6</v>
       </c>
       <c r="L41" s="5" t="n">
-        <v>5.01</v>
+        <v>6</v>
       </c>
       <c r="M41" s="6" t="n">
-        <v>1.6</v>
+        <v>128.23</v>
       </c>
       <c r="N41" s="5" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F42" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
-        <v>22.1</v>
+        <v>172.07</v>
       </c>
       <c r="J42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K42" s="5" t="n">
-        <v>5.02</v>
+        <v>7.39</v>
       </c>
       <c r="L42" s="5" t="n">
-        <v>5.02</v>
+        <v>7.39</v>
       </c>
       <c r="M42" s="6" t="n">
-        <v>1.11</v>
+        <v>12.72</v>
       </c>
       <c r="N42" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B43" s="3" t="s"/>
       <c r="C43" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>27</v>
@@ -2124,69 +2114,67 @@
         <v>45170</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="H43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
-        <v>8.46</v>
+        <v>1</v>
       </c>
       <c r="J43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="5" t="n">
-        <v>5.91</v>
+        <v>8</v>
       </c>
       <c r="L43" s="5" t="n">
-        <v>5.91</v>
+        <v>8</v>
       </c>
       <c r="M43" s="6" t="n">
-        <v>0.5</v>
+        <v>0.08</v>
       </c>
       <c r="N43" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s"/>
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F44" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
-        <v>6.57</v>
+        <v>282</v>
       </c>
       <c r="J44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K44" s="5" t="n">
-        <v>5.94</v>
+        <v>6.85</v>
       </c>
       <c r="L44" s="5" t="n">
-        <v>5.94</v>
+        <v>6.85</v>
       </c>
       <c r="M44" s="6" t="n">
-        <v>0.39</v>
+        <v>19.32</v>
       </c>
       <c r="N44" s="5" t="n">
         <v>1</v>
@@ -2194,46 +2182,46 @@
     </row>
     <row r="45" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F45" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
-        <v>37.18</v>
+        <v>73.57</v>
       </c>
       <c r="J45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="5" t="n">
-        <v>5.97</v>
+        <v>6.01</v>
       </c>
       <c r="L45" s="5" t="n">
-        <v>5.97</v>
+        <v>6.01</v>
       </c>
       <c r="M45" s="6" t="n">
-        <v>2.22</v>
+        <v>4.42</v>
       </c>
       <c r="N45" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -2241,40 +2229,40 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F46" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
-        <v>20.25</v>
+        <v>42.24</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K46" s="5" t="n">
-        <v>5.98</v>
+        <v>5</v>
       </c>
       <c r="L46" s="5" t="n">
-        <v>5.98</v>
+        <v>5</v>
       </c>
       <c r="M46" s="6" t="n">
-        <v>1.21</v>
+        <v>2.11</v>
       </c>
       <c r="N46" s="5" t="n">
         <v>1</v>
@@ -2282,75 +2270,75 @@
     </row>
     <row r="47" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F47" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
-        <v>266.69</v>
+        <v>68.38</v>
       </c>
       <c r="J47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K47" s="5" t="n">
-        <v>5.99</v>
+        <v>9.07</v>
       </c>
       <c r="L47" s="5" t="n">
-        <v>5.99</v>
+        <v>9.07</v>
       </c>
       <c r="M47" s="6" t="n">
-        <v>15.97</v>
+        <v>6.2</v>
       </c>
       <c r="N47" s="5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F48" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
-        <v>2137.12</v>
+        <v>1136</v>
       </c>
       <c r="J48" s="5" t="n">
         <v>0</v>
@@ -2362,112 +2350,108 @@
         <v>6</v>
       </c>
       <c r="M48" s="6" t="n">
-        <v>128.23</v>
+        <v>68.16</v>
       </c>
       <c r="N48" s="5" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B49" s="3" t="s"/>
       <c r="C49" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F49" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I49" s="6" t="n">
-        <v>152.11</v>
+        <v>82.34</v>
       </c>
       <c r="J49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K49" s="5" t="n">
-        <v>6.01</v>
+        <v>6.5</v>
       </c>
       <c r="L49" s="5" t="n">
-        <v>6.01</v>
+        <v>6.5</v>
       </c>
       <c r="M49" s="6" t="n">
-        <v>9.14</v>
+        <v>5.35</v>
       </c>
       <c r="N49" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F50" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I50" s="6" t="n">
-        <v>62.32</v>
+        <v>6.22</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K50" s="5" t="n">
-        <v>6.02</v>
+        <v>5.95</v>
       </c>
       <c r="L50" s="5" t="n">
-        <v>6.02</v>
+        <v>5.95</v>
       </c>
       <c r="M50" s="6" t="n">
-        <v>3.75</v>
+        <v>0.37</v>
       </c>
       <c r="N50" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B51" s="3" t="s"/>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>27</v>
@@ -2476,153 +2460,155 @@
         <v>45170</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I51" s="6" t="n">
-        <v>40.29</v>
+        <v>2182.39</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K51" s="5" t="n">
-        <v>6.03</v>
+        <v>7.9</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>6.03</v>
+        <v>7.9</v>
       </c>
       <c r="M51" s="6" t="n">
-        <v>2.43</v>
+        <v>172.41</v>
       </c>
       <c r="N51" s="5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="F52" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="H52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
-        <v>145.29</v>
+        <v>0.99</v>
       </c>
       <c r="J52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="5" t="n">
-        <v>6.8</v>
+        <v>6.06</v>
       </c>
       <c r="L52" s="5" t="n">
-        <v>6.8</v>
+        <v>6.06</v>
       </c>
       <c r="M52" s="6" t="n">
-        <v>9.88</v>
+        <v>0.06</v>
       </c>
       <c r="N52" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B53" s="3" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F53" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
-        <v>4.79</v>
+        <v>8.46</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K53" s="5" t="n">
-        <v>5.85</v>
+        <v>5.91</v>
       </c>
       <c r="L53" s="5" t="n">
-        <v>5.85</v>
+        <v>5.91</v>
       </c>
       <c r="M53" s="6" t="n">
-        <v>0.28</v>
+        <v>0.5</v>
       </c>
       <c r="N53" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B54" s="3" t="s"/>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F54" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H54" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I54" s="6" t="n">
-        <v>25.47</v>
+        <v>3.71</v>
       </c>
       <c r="J54" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K54" s="5" t="n">
-        <v>5.89</v>
+        <v>2.7</v>
       </c>
       <c r="L54" s="5" t="n">
-        <v>5.89</v>
+        <v>0.3</v>
       </c>
       <c r="M54" s="6" t="n">
-        <v>1.5</v>
+        <v>0.01</v>
       </c>
       <c r="N54" s="5" t="n">
         <v>1</v>
@@ -2630,41 +2616,43 @@
     </row>
     <row r="55" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="3" t="s"/>
+        <v>43</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C55" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F55" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I55" s="6" t="n">
-        <v>12.71</v>
+        <v>69.44</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="5" t="n">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="L55" s="5" t="n">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="M55" s="6" t="n">
-        <v>0.75</v>
+        <v>4.79</v>
       </c>
       <c r="N55" s="5" t="n">
         <v>1</v>
@@ -2672,125 +2660,129 @@
     </row>
     <row r="56" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="3" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C56" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="H56" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I56" s="6" t="n">
-        <v>33</v>
+        <v>121.15</v>
       </c>
       <c r="J56" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K56" s="5" t="n">
-        <v>5.91</v>
+        <v>5.99</v>
       </c>
       <c r="L56" s="5" t="n">
-        <v>5.91</v>
+        <v>5.99</v>
       </c>
       <c r="M56" s="6" t="n">
-        <v>1.95</v>
+        <v>7.26</v>
       </c>
       <c r="N56" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="3" t="s"/>
+        <v>22</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C57" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F57" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="H57" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I57" s="6" t="n">
-        <v>7.76</v>
+        <v>33.9</v>
       </c>
       <c r="J57" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K57" s="5" t="n">
-        <v>5.93</v>
+        <v>6.02</v>
       </c>
       <c r="L57" s="5" t="n">
-        <v>5.93</v>
+        <v>6.02</v>
       </c>
       <c r="M57" s="6" t="n">
-        <v>0.46</v>
+        <v>2.04</v>
       </c>
       <c r="N57" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B58" s="3" t="s"/>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F58" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I58" s="6" t="n">
-        <v>9.59</v>
+        <v>26</v>
       </c>
       <c r="J58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K58" s="5" t="n">
-        <v>5.94</v>
+        <v>7.88</v>
       </c>
       <c r="L58" s="5" t="n">
-        <v>5.94</v>
+        <v>7.88</v>
       </c>
       <c r="M58" s="6" t="n">
-        <v>0.57</v>
+        <v>2.05</v>
       </c>
       <c r="N58" s="5" t="n">
         <v>1</v>
@@ -2798,41 +2790,43 @@
     </row>
     <row r="59" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="3" t="s"/>
+        <v>43</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C59" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F59" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H59" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I59" s="6" t="n">
-        <v>26</v>
+        <v>0.01</v>
       </c>
       <c r="J59" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="5" t="n">
-        <v>7.88</v>
+        <v>0</v>
       </c>
       <c r="L59" s="5" t="n">
-        <v>7.88</v>
+        <v>0</v>
       </c>
       <c r="M59" s="6" t="n">
-        <v>2.05</v>
+        <v>0</v>
       </c>
       <c r="N59" s="5" t="n">
         <v>1</v>
@@ -2840,98 +2834,100 @@
     </row>
     <row r="60" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B60" s="3" t="s"/>
       <c r="C60" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F60" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H60" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I60" s="6" t="n">
-        <v>42.58</v>
+        <v>1.19</v>
       </c>
       <c r="J60" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="5" t="n">
-        <v>7.89</v>
+        <v>5.04</v>
       </c>
       <c r="L60" s="5" t="n">
-        <v>7.89</v>
+        <v>5.04</v>
       </c>
       <c r="M60" s="6" t="n">
-        <v>3.36</v>
+        <v>0.06</v>
       </c>
       <c r="N60" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="3" t="s"/>
+        <v>32</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C61" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F61" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H61" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I61" s="6" t="n">
-        <v>2182.39</v>
+        <v>10.99</v>
       </c>
       <c r="J61" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="5" t="n">
-        <v>7.9</v>
+        <v>7.37</v>
       </c>
       <c r="L61" s="5" t="n">
-        <v>7.9</v>
+        <v>7.37</v>
       </c>
       <c r="M61" s="6" t="n">
-        <v>172.41</v>
+        <v>0.81</v>
       </c>
       <c r="N61" s="5" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B62" s="3" t="s"/>
       <c r="C62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>46</v>
@@ -2946,61 +2942,61 @@
         <v>0</v>
       </c>
       <c r="I62" s="6" t="n">
-        <v>75.74</v>
+        <v>9.99</v>
       </c>
       <c r="J62" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K62" s="5" t="n">
-        <v>7.91</v>
+        <v>6.81</v>
       </c>
       <c r="L62" s="5" t="n">
-        <v>7.91</v>
+        <v>6.81</v>
       </c>
       <c r="M62" s="6" t="n">
-        <v>5.99</v>
+        <v>0.68</v>
       </c>
       <c r="N62" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B63" s="3" t="s"/>
       <c r="C63" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F63" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H63" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I63" s="6" t="n">
-        <v>19.56</v>
+        <v>7.76</v>
       </c>
       <c r="J63" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K63" s="5" t="n">
-        <v>7.92</v>
+        <v>5.93</v>
       </c>
       <c r="L63" s="5" t="n">
-        <v>7.92</v>
+        <v>5.93</v>
       </c>
       <c r="M63" s="6" t="n">
-        <v>1.55</v>
+        <v>0.46</v>
       </c>
       <c r="N63" s="5" t="n">
         <v>1</v>
@@ -3008,41 +3004,43 @@
     </row>
     <row r="64" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="3" t="s"/>
+        <v>22</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C64" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F64" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="H64" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I64" s="6" t="n">
-        <v>1</v>
+        <v>40.42</v>
       </c>
       <c r="J64" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K64" s="5" t="n">
-        <v>8</v>
+        <v>6.01</v>
       </c>
       <c r="L64" s="5" t="n">
-        <v>8</v>
+        <v>6.01</v>
       </c>
       <c r="M64" s="6" t="n">
-        <v>0.08</v>
+        <v>2.43</v>
       </c>
       <c r="N64" s="5" t="n">
         <v>1</v>
@@ -3050,41 +3048,43 @@
     </row>
     <row r="65" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="3" t="s"/>
+        <v>32</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C65" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F65" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H65" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I65" s="6" t="n">
-        <v>2.49</v>
+        <v>28.92</v>
       </c>
       <c r="J65" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K65" s="5" t="n">
-        <v>8.03</v>
+        <v>7.4</v>
       </c>
       <c r="L65" s="5" t="n">
-        <v>8.03</v>
+        <v>7.4</v>
       </c>
       <c r="M65" s="6" t="n">
-        <v>0.2</v>
+        <v>2.14</v>
       </c>
       <c r="N65" s="5" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Alterações na tela conferencia de vendas
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação de Taxas.xlsx
+++ b/cypress/downloads/Conciliação de Taxas.xlsx
@@ -59,106 +59,106 @@
     <t>Qtde.</t>
   </si>
   <si>
+    <t>013998257000126</t>
+  </si>
+  <si>
+    <t>82123891000138</t>
+  </si>
+  <si>
+    <t>EMPRESA MODELO</t>
+  </si>
+  <si>
+    <t>Valecard</t>
+  </si>
+  <si>
+    <t>Valecard Voucher</t>
+  </si>
+  <si>
+    <t>033091040000145</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>VR REFEICAO</t>
+  </si>
+  <si>
+    <t>Sodexo</t>
+  </si>
+  <si>
+    <t>SODEXO REFEICAO</t>
+  </si>
+  <si>
+    <t>033090890000129</t>
+  </si>
+  <si>
+    <t>000000080683312</t>
+  </si>
+  <si>
+    <t>000000008784337</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>TICKET ALIMENTACAO</t>
+  </si>
+  <si>
+    <t>000000008784329</t>
+  </si>
+  <si>
+    <t>TICKET REFEICAO</t>
+  </si>
+  <si>
     <t>000000080683215</t>
   </si>
   <si>
+    <t>000000008781044</t>
+  </si>
+  <si>
+    <t>000000008781052</t>
+  </si>
+  <si>
+    <t>Cabal</t>
+  </si>
+  <si>
+    <t>CABAL VOUCHER</t>
+  </si>
+  <si>
+    <t>000000007815066</t>
+  </si>
+  <si>
+    <t>UpBrasil</t>
+  </si>
+  <si>
+    <t>UpBrasil Convênio</t>
+  </si>
+  <si>
+    <t>000000007815071</t>
+  </si>
+  <si>
     <t>000000012784869</t>
   </si>
   <si>
-    <t>82123891000138</t>
-  </si>
-  <si>
-    <t>EMPRESA MODELO</t>
-  </si>
-  <si>
-    <t>Ticket</t>
-  </si>
-  <si>
     <t>Ticket Flex</t>
   </si>
   <si>
-    <t>000000008781044</t>
-  </si>
-  <si>
-    <t>TICKET ALIMENTACAO</t>
-  </si>
-  <si>
-    <t>000000080683312</t>
-  </si>
-  <si>
-    <t>000000008784337</t>
-  </si>
-  <si>
-    <t>033090890000129</t>
-  </si>
-  <si>
-    <t>Sodexo</t>
-  </si>
-  <si>
-    <t>SODEXO REFEICAO</t>
+    <t>000000001438301</t>
+  </si>
+  <si>
+    <t>000000000143830</t>
+  </si>
+  <si>
+    <t>Green Card</t>
+  </si>
+  <si>
+    <t>Green Card Débito</t>
   </si>
   <si>
     <t>Comprocard</t>
   </si>
   <si>
     <t>Comprocard Crédito</t>
-  </si>
-  <si>
-    <t>000000008784329</t>
-  </si>
-  <si>
-    <t>TICKET REFEICAO</t>
-  </si>
-  <si>
-    <t>000000007815071</t>
-  </si>
-  <si>
-    <t>000000007815066</t>
-  </si>
-  <si>
-    <t>UpBrasil</t>
-  </si>
-  <si>
-    <t>UpBrasil Convênio</t>
-  </si>
-  <si>
-    <t>013998257000126</t>
-  </si>
-  <si>
-    <t>Valecard</t>
-  </si>
-  <si>
-    <t>Valecard Voucher</t>
-  </si>
-  <si>
-    <t>000000001438301</t>
-  </si>
-  <si>
-    <t>000000000143830</t>
-  </si>
-  <si>
-    <t>Green Card</t>
-  </si>
-  <si>
-    <t>Green Card Débito</t>
-  </si>
-  <si>
-    <t>000000008781052</t>
-  </si>
-  <si>
-    <t>033091040000145</t>
-  </si>
-  <si>
-    <t>Cabal</t>
-  </si>
-  <si>
-    <t>CABAL VOUCHER</t>
-  </si>
-  <si>
-    <t>VR</t>
-  </si>
-  <si>
-    <t>VR REFEICAO</t>
   </si>
   <si>
     <t>127.811,42</t>
@@ -263,7 +263,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col width="20.57" min="1" max="1" customWidth="1"/>
-    <col width="18" min="2" max="2" customWidth="1"/>
+    <col width="17.86" min="2" max="2" customWidth="1"/>
     <col width="15.43" min="3" max="3" customWidth="1"/>
     <col width="17.71" min="4" max="4" customWidth="1"/>
     <col width="16" min="5" max="5" customWidth="1"/>
@@ -326,41 +326,39 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B2" s="3" t="s"/>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>6.57</v>
+        <v>3.71</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>5.94</v>
+        <v>2.7</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>5.94</v>
+        <v>0.3</v>
       </c>
       <c r="M2" s="6" t="n">
-        <v>0.39</v>
+        <v>0.01</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>1</v>
@@ -370,171 +368,165 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="B3" s="3" t="s"/>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>62.05</v>
+        <v>164.29</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>6.01</v>
+        <v>2.79</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>6.01</v>
+        <v>0.39</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>3.73</v>
+        <v>0.64</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s"/>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>29.75</v>
+        <v>118422.66</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>5.98</v>
+        <v>2.8</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>5.98</v>
+        <v>0.4</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>1.78</v>
+        <v>473.69</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s"/>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>15.52</v>
+        <v>133.63</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>6.89</v>
+        <v>2.81</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>6.89</v>
+        <v>0.41</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>1.07</v>
+        <v>0.55</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s"/>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v>4.79</v>
+        <v>9.99</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>5.85</v>
+        <v>6.81</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>5.85</v>
+        <v>6.81</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>0.28</v>
+        <v>0.68</v>
       </c>
       <c r="N6" s="5" t="n">
         <v>1</v>
@@ -542,19 +534,17 @@
     </row>
     <row r="7" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s"/>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>45170</v>
@@ -566,63 +556,63 @@
         <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v>299.89</v>
+        <v>282</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>6</v>
+        <v>6.85</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>6</v>
+        <v>6.85</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>17.99</v>
+        <v>19.32</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="F8" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>5.79</v>
+        <v>0.01</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>6.04</v>
+        <v>0</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>6.04</v>
+        <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="N8" s="5" t="n">
         <v>1</v>
@@ -630,43 +620,43 @@
     </row>
     <row r="9" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F9" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>150</v>
+        <v>69.44</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>9</v>
+        <v>4.79</v>
       </c>
       <c r="N9" s="5" t="n">
         <v>1</v>
@@ -674,43 +664,43 @@
     </row>
     <row r="10" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>31.95</v>
+        <v>15.52</v>
       </c>
       <c r="J10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>5.01</v>
+        <v>6.89</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>5.01</v>
+        <v>6.89</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>1.6</v>
+        <v>1.07</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>1</v>
@@ -718,56 +708,60 @@
     </row>
     <row r="11" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="3" t="s"/>
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="6" t="n">
-        <v>164.29</v>
+        <v>6.22</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>2.79</v>
+        <v>5.95</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>0.39</v>
+        <v>5.95</v>
       </c>
       <c r="M11" s="6" t="n">
-        <v>0.64</v>
+        <v>0.37</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s"/>
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>27</v>
@@ -782,19 +776,19 @@
         <v>0</v>
       </c>
       <c r="I12" s="6" t="n">
-        <v>9.59</v>
+        <v>29.75</v>
       </c>
       <c r="J12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>5.94</v>
+        <v>5.98</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>5.94</v>
+        <v>5.98</v>
       </c>
       <c r="M12" s="6" t="n">
-        <v>0.57</v>
+        <v>1.78</v>
       </c>
       <c r="N12" s="5" t="n">
         <v>1</v>
@@ -802,190 +796,192 @@
     </row>
     <row r="13" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="6" t="n">
-        <v>145.29</v>
+        <v>174.71</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>6.8</v>
+        <v>5.99</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>6.8</v>
+        <v>5.99</v>
       </c>
       <c r="M13" s="6" t="n">
-        <v>9.88</v>
+        <v>10.47</v>
       </c>
       <c r="N13" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="6" t="n">
-        <v>58.01</v>
+        <v>1136</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>7.38</v>
+        <v>6</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>7.38</v>
+        <v>6</v>
       </c>
       <c r="M14" s="6" t="n">
-        <v>4.28</v>
+        <v>68.16</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="6" t="n">
-        <v>266.69</v>
+        <v>104.65</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>5.99</v>
+        <v>6.01</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>5.99</v>
+        <v>6.01</v>
       </c>
       <c r="M15" s="6" t="n">
-        <v>15.97</v>
+        <v>6.29</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="6" t="n">
-        <v>490.6</v>
+        <v>33.9</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="5" t="n">
-        <v>6</v>
+        <v>6.02</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>6</v>
+        <v>6.02</v>
       </c>
       <c r="M16" s="6" t="n">
-        <v>29.44</v>
+        <v>2.04</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s"/>
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>27</v>
@@ -1000,19 +996,19 @@
         <v>0</v>
       </c>
       <c r="I17" s="6" t="n">
-        <v>12.71</v>
+        <v>5.79</v>
       </c>
       <c r="J17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>5.9</v>
+        <v>6.04</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>5.9</v>
+        <v>6.04</v>
       </c>
       <c r="M17" s="6" t="n">
-        <v>0.75</v>
+        <v>0.35</v>
       </c>
       <c r="N17" s="5" t="n">
         <v>1</v>
@@ -1020,163 +1016,163 @@
     </row>
     <row r="18" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="6" t="n">
-        <v>174.71</v>
+        <v>0.99</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>5.99</v>
+        <v>6.06</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>5.99</v>
+        <v>6.06</v>
       </c>
       <c r="M18" s="6" t="n">
-        <v>10.47</v>
+        <v>0.06</v>
       </c>
       <c r="N18" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="6" t="n">
-        <v>51.86</v>
+        <v>0.02</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>6.02</v>
+        <v>0</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>6.02</v>
+        <v>0</v>
       </c>
       <c r="M19" s="6" t="n">
-        <v>3.12</v>
+        <v>0</v>
       </c>
       <c r="N19" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="6" t="n">
-        <v>62.32</v>
+        <v>150</v>
       </c>
       <c r="J20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>6.02</v>
+        <v>6</v>
       </c>
       <c r="L20" s="5" t="n">
-        <v>6.02</v>
+        <v>6</v>
       </c>
       <c r="M20" s="6" t="n">
-        <v>3.75</v>
+        <v>9</v>
       </c>
       <c r="N20" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="6" t="n">
-        <v>152.11</v>
+        <v>40.42</v>
       </c>
       <c r="J21" s="5" t="n">
         <v>0</v>
@@ -1188,22 +1184,24 @@
         <v>6.01</v>
       </c>
       <c r="M21" s="6" t="n">
-        <v>9.14</v>
+        <v>2.43</v>
       </c>
       <c r="N21" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>27</v>
@@ -1218,34 +1216,36 @@
         <v>0</v>
       </c>
       <c r="I22" s="6" t="n">
-        <v>75.74</v>
+        <v>9.19</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>7.91</v>
+        <v>5.98</v>
       </c>
       <c r="L22" s="5" t="n">
-        <v>7.91</v>
+        <v>5.98</v>
       </c>
       <c r="M22" s="6" t="n">
-        <v>5.99</v>
+        <v>0.55</v>
       </c>
       <c r="N22" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>27</v>
@@ -1260,195 +1260,195 @@
         <v>0</v>
       </c>
       <c r="I23" s="6" t="n">
-        <v>25.47</v>
+        <v>121.15</v>
       </c>
       <c r="J23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>5.89</v>
+        <v>5.99</v>
       </c>
       <c r="L23" s="5" t="n">
-        <v>5.89</v>
+        <v>5.99</v>
       </c>
       <c r="M23" s="6" t="n">
-        <v>1.5</v>
+        <v>7.26</v>
       </c>
       <c r="N23" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="6" t="n">
-        <v>6.08</v>
+        <v>299.89</v>
       </c>
       <c r="J24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K24" s="5" t="n">
-        <v>5.92</v>
+        <v>6</v>
       </c>
       <c r="L24" s="5" t="n">
-        <v>5.92</v>
+        <v>6</v>
       </c>
       <c r="M24" s="6" t="n">
-        <v>0.36</v>
+        <v>17.99</v>
       </c>
       <c r="N24" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="6" t="n">
-        <v>20.25</v>
+        <v>62.05</v>
       </c>
       <c r="J25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K25" s="5" t="n">
-        <v>5.98</v>
+        <v>6.01</v>
       </c>
       <c r="L25" s="5" t="n">
-        <v>5.98</v>
+        <v>6.01</v>
       </c>
       <c r="M25" s="6" t="n">
-        <v>1.21</v>
+        <v>3.73</v>
       </c>
       <c r="N25" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="6" t="n">
-        <v>40.29</v>
+        <v>51.86</v>
       </c>
       <c r="J26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K26" s="5" t="n">
-        <v>6.03</v>
+        <v>6.02</v>
       </c>
       <c r="L26" s="5" t="n">
-        <v>6.03</v>
+        <v>6.02</v>
       </c>
       <c r="M26" s="6" t="n">
-        <v>2.43</v>
+        <v>3.12</v>
       </c>
       <c r="N26" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="6" t="n">
-        <v>9.19</v>
+        <v>6.08</v>
       </c>
       <c r="J27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K27" s="5" t="n">
-        <v>5.98</v>
+        <v>5.92</v>
       </c>
       <c r="L27" s="5" t="n">
-        <v>5.98</v>
+        <v>5.92</v>
       </c>
       <c r="M27" s="6" t="n">
-        <v>0.55</v>
+        <v>0.36</v>
       </c>
       <c r="N27" s="5" t="n">
         <v>1</v>
@@ -1456,61 +1456,63 @@
     </row>
     <row r="28" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F28" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H28" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="6" t="n">
-        <v>133.63</v>
+        <v>490.6</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K28" s="5" t="n">
-        <v>2.81</v>
+        <v>6</v>
       </c>
       <c r="L28" s="5" t="n">
-        <v>0.41</v>
+        <v>6</v>
       </c>
       <c r="M28" s="6" t="n">
-        <v>0.55</v>
+        <v>29.44</v>
       </c>
       <c r="N28" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>45170</v>
@@ -1522,19 +1524,19 @@
         <v>0</v>
       </c>
       <c r="I29" s="6" t="n">
-        <v>0.02</v>
+        <v>73.57</v>
       </c>
       <c r="J29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="5" t="n">
-        <v>0</v>
+        <v>6.01</v>
       </c>
       <c r="L29" s="5" t="n">
-        <v>0</v>
+        <v>6.01</v>
       </c>
       <c r="M29" s="6" t="n">
-        <v>0</v>
+        <v>4.42</v>
       </c>
       <c r="N29" s="5" t="n">
         <v>2</v>
@@ -1542,85 +1544,83 @@
     </row>
     <row r="30" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B30" s="3" t="s"/>
       <c r="C30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="6" t="n">
-        <v>104.65</v>
+        <v>4.98</v>
       </c>
       <c r="J30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K30" s="5" t="n">
-        <v>6.01</v>
+        <v>5.02</v>
       </c>
       <c r="L30" s="5" t="n">
-        <v>6.01</v>
+        <v>5.02</v>
       </c>
       <c r="M30" s="6" t="n">
-        <v>6.29</v>
+        <v>0.25</v>
       </c>
       <c r="N30" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B31" s="3" t="s"/>
       <c r="C31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="6" t="n">
-        <v>2.49</v>
+        <v>1.19</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K31" s="5" t="n">
-        <v>8.03</v>
+        <v>5.04</v>
       </c>
       <c r="L31" s="5" t="n">
-        <v>8.03</v>
+        <v>5.04</v>
       </c>
       <c r="M31" s="6" t="n">
-        <v>0.2</v>
+        <v>0.06</v>
       </c>
       <c r="N31" s="5" t="n">
         <v>1</v>
@@ -1628,46 +1628,44 @@
     </row>
     <row r="32" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B32" s="3" t="s"/>
       <c r="C32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="6" t="n">
-        <v>37.18</v>
+        <v>31.15</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="5" t="n">
-        <v>5.97</v>
+        <v>6.48</v>
       </c>
       <c r="L32" s="5" t="n">
-        <v>5.97</v>
+        <v>6.48</v>
       </c>
       <c r="M32" s="6" t="n">
-        <v>2.22</v>
+        <v>2.02</v>
       </c>
       <c r="N32" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -1676,37 +1674,37 @@
       </c>
       <c r="B33" s="3" t="s"/>
       <c r="C33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I33" s="6" t="n">
-        <v>39.65</v>
+        <v>82.34</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="5" t="n">
-        <v>6.51</v>
+        <v>6.5</v>
       </c>
       <c r="L33" s="5" t="n">
-        <v>6.51</v>
+        <v>6.5</v>
       </c>
       <c r="M33" s="6" t="n">
-        <v>2.58</v>
+        <v>5.35</v>
       </c>
       <c r="N33" s="5" t="n">
         <v>1</v>
@@ -1718,37 +1716,37 @@
       </c>
       <c r="B34" s="3" t="s"/>
       <c r="C34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="n">
-        <v>4.98</v>
+        <v>39.65</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="5" t="n">
-        <v>5.02</v>
+        <v>6.51</v>
       </c>
       <c r="L34" s="5" t="n">
-        <v>5.02</v>
+        <v>6.51</v>
       </c>
       <c r="M34" s="6" t="n">
-        <v>0.25</v>
+        <v>2.58</v>
       </c>
       <c r="N34" s="5" t="n">
         <v>1</v>
@@ -1756,83 +1754,87 @@
     </row>
     <row r="35" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="3" t="s"/>
+        <v>36</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="n">
-        <v>118422.66</v>
+        <v>10.99</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K35" s="5" t="n">
-        <v>2.8</v>
+        <v>7.37</v>
       </c>
       <c r="L35" s="5" t="n">
-        <v>0.4</v>
+        <v>7.37</v>
       </c>
       <c r="M35" s="6" t="n">
-        <v>473.69</v>
+        <v>0.81</v>
       </c>
       <c r="N35" s="5" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="3" t="s"/>
+        <v>36</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I36" s="6" t="n">
-        <v>42.58</v>
+        <v>58.01</v>
       </c>
       <c r="J36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K36" s="5" t="n">
-        <v>7.89</v>
+        <v>7.38</v>
       </c>
       <c r="L36" s="5" t="n">
-        <v>7.89</v>
+        <v>7.38</v>
       </c>
       <c r="M36" s="6" t="n">
-        <v>3.36</v>
+        <v>4.28</v>
       </c>
       <c r="N36" s="5" t="n">
         <v>2</v>
@@ -1840,85 +1842,87 @@
     </row>
     <row r="37" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="3" t="s"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F37" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I37" s="6" t="n">
-        <v>33</v>
+        <v>172.07</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K37" s="5" t="n">
-        <v>5.91</v>
+        <v>7.39</v>
       </c>
       <c r="L37" s="5" t="n">
-        <v>5.91</v>
+        <v>7.39</v>
       </c>
       <c r="M37" s="6" t="n">
-        <v>1.95</v>
+        <v>12.72</v>
       </c>
       <c r="N37" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F38" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I38" s="6" t="n">
-        <v>22.1</v>
+        <v>28.92</v>
       </c>
       <c r="J38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K38" s="5" t="n">
-        <v>5.02</v>
+        <v>7.4</v>
       </c>
       <c r="L38" s="5" t="n">
-        <v>5.02</v>
+        <v>7.4</v>
       </c>
       <c r="M38" s="6" t="n">
-        <v>1.11</v>
+        <v>2.14</v>
       </c>
       <c r="N38" s="5" t="n">
         <v>1</v>
@@ -1926,83 +1930,87 @@
     </row>
     <row r="39" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="3" t="s"/>
+        <v>36</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I39" s="6" t="n">
-        <v>19.56</v>
+        <v>68.38</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>7.92</v>
+        <v>9.07</v>
       </c>
       <c r="L39" s="5" t="n">
-        <v>7.92</v>
+        <v>9.07</v>
       </c>
       <c r="M39" s="6" t="n">
-        <v>1.55</v>
+        <v>6.2</v>
       </c>
       <c r="N39" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="3" t="s"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="6" t="n">
-        <v>31.15</v>
+        <v>42.24</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K40" s="5" t="n">
-        <v>6.48</v>
+        <v>5</v>
       </c>
       <c r="L40" s="5" t="n">
-        <v>6.48</v>
+        <v>5</v>
       </c>
       <c r="M40" s="6" t="n">
-        <v>2.02</v>
+        <v>2.11</v>
       </c>
       <c r="N40" s="5" t="n">
         <v>1</v>
@@ -2010,102 +2018,104 @@
     </row>
     <row r="41" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F41" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="6" t="n">
-        <v>2137.12</v>
+        <v>31.95</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>6</v>
+        <v>5.01</v>
       </c>
       <c r="L41" s="5" t="n">
-        <v>6</v>
+        <v>5.01</v>
       </c>
       <c r="M41" s="6" t="n">
-        <v>128.23</v>
+        <v>1.6</v>
       </c>
       <c r="N41" s="5" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F42" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
-        <v>172.07</v>
+        <v>22.1</v>
       </c>
       <c r="J42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K42" s="5" t="n">
-        <v>7.39</v>
+        <v>5.02</v>
       </c>
       <c r="L42" s="5" t="n">
-        <v>7.39</v>
+        <v>5.02</v>
       </c>
       <c r="M42" s="6" t="n">
-        <v>12.72</v>
+        <v>1.11</v>
       </c>
       <c r="N42" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>27</v>
@@ -2114,67 +2124,69 @@
         <v>45170</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
-        <v>1</v>
+        <v>8.46</v>
       </c>
       <c r="J43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="5" t="n">
-        <v>8</v>
+        <v>5.91</v>
       </c>
       <c r="L43" s="5" t="n">
-        <v>8</v>
+        <v>5.91</v>
       </c>
       <c r="M43" s="6" t="n">
-        <v>0.08</v>
+        <v>0.5</v>
       </c>
       <c r="N43" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F44" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
-        <v>282</v>
+        <v>6.57</v>
       </c>
       <c r="J44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K44" s="5" t="n">
-        <v>6.85</v>
+        <v>5.94</v>
       </c>
       <c r="L44" s="5" t="n">
-        <v>6.85</v>
+        <v>5.94</v>
       </c>
       <c r="M44" s="6" t="n">
-        <v>19.32</v>
+        <v>0.39</v>
       </c>
       <c r="N44" s="5" t="n">
         <v>1</v>
@@ -2182,46 +2194,46 @@
     </row>
     <row r="45" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F45" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
-        <v>73.57</v>
+        <v>37.18</v>
       </c>
       <c r="J45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="5" t="n">
-        <v>6.01</v>
+        <v>5.97</v>
       </c>
       <c r="L45" s="5" t="n">
-        <v>6.01</v>
+        <v>5.97</v>
       </c>
       <c r="M45" s="6" t="n">
-        <v>4.42</v>
+        <v>2.22</v>
       </c>
       <c r="N45" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -2229,40 +2241,40 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F46" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
-        <v>42.24</v>
+        <v>20.25</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K46" s="5" t="n">
-        <v>5</v>
+        <v>5.98</v>
       </c>
       <c r="L46" s="5" t="n">
-        <v>5</v>
+        <v>5.98</v>
       </c>
       <c r="M46" s="6" t="n">
-        <v>2.11</v>
+        <v>1.21</v>
       </c>
       <c r="N46" s="5" t="n">
         <v>1</v>
@@ -2270,75 +2282,75 @@
     </row>
     <row r="47" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F47" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
-        <v>68.38</v>
+        <v>266.69</v>
       </c>
       <c r="J47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K47" s="5" t="n">
-        <v>9.07</v>
+        <v>5.99</v>
       </c>
       <c r="L47" s="5" t="n">
-        <v>9.07</v>
+        <v>5.99</v>
       </c>
       <c r="M47" s="6" t="n">
-        <v>6.2</v>
+        <v>15.97</v>
       </c>
       <c r="N47" s="5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F48" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
-        <v>1136</v>
+        <v>2137.12</v>
       </c>
       <c r="J48" s="5" t="n">
         <v>0</v>
@@ -2350,108 +2362,112 @@
         <v>6</v>
       </c>
       <c r="M48" s="6" t="n">
-        <v>68.16</v>
+        <v>128.23</v>
       </c>
       <c r="N48" s="5" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F49" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I49" s="6" t="n">
-        <v>82.34</v>
+        <v>152.11</v>
       </c>
       <c r="J49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K49" s="5" t="n">
-        <v>6.5</v>
+        <v>6.01</v>
       </c>
       <c r="L49" s="5" t="n">
-        <v>6.5</v>
+        <v>6.01</v>
       </c>
       <c r="M49" s="6" t="n">
-        <v>5.35</v>
+        <v>9.14</v>
       </c>
       <c r="N49" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F50" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I50" s="6" t="n">
-        <v>6.22</v>
+        <v>62.32</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K50" s="5" t="n">
-        <v>5.95</v>
+        <v>6.02</v>
       </c>
       <c r="L50" s="5" t="n">
-        <v>5.95</v>
+        <v>6.02</v>
       </c>
       <c r="M50" s="6" t="n">
-        <v>0.37</v>
+        <v>3.75</v>
       </c>
       <c r="N50" s="5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>27</v>
@@ -2460,155 +2476,153 @@
         <v>45170</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I51" s="6" t="n">
-        <v>2182.39</v>
+        <v>40.29</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K51" s="5" t="n">
-        <v>7.9</v>
+        <v>6.03</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>7.9</v>
+        <v>6.03</v>
       </c>
       <c r="M51" s="6" t="n">
-        <v>172.41</v>
+        <v>2.43</v>
       </c>
       <c r="N51" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F52" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
-        <v>0.99</v>
+        <v>145.29</v>
       </c>
       <c r="J52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="5" t="n">
-        <v>6.06</v>
+        <v>6.8</v>
       </c>
       <c r="L52" s="5" t="n">
-        <v>6.06</v>
+        <v>6.8</v>
       </c>
       <c r="M52" s="6" t="n">
-        <v>0.06</v>
+        <v>9.88</v>
       </c>
       <c r="N52" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B53" s="3" t="s"/>
       <c r="C53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F53" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
-        <v>8.46</v>
+        <v>4.79</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K53" s="5" t="n">
-        <v>5.91</v>
+        <v>5.85</v>
       </c>
       <c r="L53" s="5" t="n">
-        <v>5.91</v>
+        <v>5.85</v>
       </c>
       <c r="M53" s="6" t="n">
-        <v>0.5</v>
+        <v>0.28</v>
       </c>
       <c r="N53" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B54" s="3" t="s"/>
       <c r="C54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F54" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H54" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I54" s="6" t="n">
-        <v>3.71</v>
+        <v>25.47</v>
       </c>
       <c r="J54" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K54" s="5" t="n">
-        <v>2.7</v>
+        <v>5.89</v>
       </c>
       <c r="L54" s="5" t="n">
-        <v>0.3</v>
+        <v>5.89</v>
       </c>
       <c r="M54" s="6" t="n">
-        <v>0.01</v>
+        <v>1.5</v>
       </c>
       <c r="N54" s="5" t="n">
         <v>1</v>
@@ -2616,43 +2630,41 @@
     </row>
     <row r="55" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B55" s="3" t="s"/>
       <c r="C55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F55" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="H55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I55" s="6" t="n">
-        <v>69.44</v>
+        <v>12.71</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="5" t="n">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="L55" s="5" t="n">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="M55" s="6" t="n">
-        <v>4.79</v>
+        <v>0.75</v>
       </c>
       <c r="N55" s="5" t="n">
         <v>1</v>
@@ -2660,129 +2672,125 @@
     </row>
     <row r="56" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B56" s="3" t="s"/>
       <c r="C56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H56" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I56" s="6" t="n">
-        <v>121.15</v>
+        <v>33</v>
       </c>
       <c r="J56" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K56" s="5" t="n">
-        <v>5.99</v>
+        <v>5.91</v>
       </c>
       <c r="L56" s="5" t="n">
-        <v>5.99</v>
+        <v>5.91</v>
       </c>
       <c r="M56" s="6" t="n">
-        <v>7.26</v>
+        <v>1.95</v>
       </c>
       <c r="N56" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B57" s="3" t="s"/>
       <c r="C57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F57" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H57" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I57" s="6" t="n">
-        <v>33.9</v>
+        <v>7.76</v>
       </c>
       <c r="J57" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K57" s="5" t="n">
-        <v>6.02</v>
+        <v>5.93</v>
       </c>
       <c r="L57" s="5" t="n">
-        <v>6.02</v>
+        <v>5.93</v>
       </c>
       <c r="M57" s="6" t="n">
-        <v>2.04</v>
+        <v>0.46</v>
       </c>
       <c r="N57" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B58" s="3" t="s"/>
       <c r="C58" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F58" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="H58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I58" s="6" t="n">
-        <v>26</v>
+        <v>9.59</v>
       </c>
       <c r="J58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K58" s="5" t="n">
-        <v>7.88</v>
+        <v>5.94</v>
       </c>
       <c r="L58" s="5" t="n">
-        <v>7.88</v>
+        <v>5.94</v>
       </c>
       <c r="M58" s="6" t="n">
-        <v>2.05</v>
+        <v>0.57</v>
       </c>
       <c r="N58" s="5" t="n">
         <v>1</v>
@@ -2790,43 +2798,41 @@
     </row>
     <row r="59" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B59" s="3" t="s"/>
       <c r="C59" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F59" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="H59" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" s="6" t="n">
-        <v>0.01</v>
-      </c>
       <c r="J59" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="5" t="n">
-        <v>0</v>
+        <v>7.88</v>
       </c>
       <c r="L59" s="5" t="n">
-        <v>0</v>
+        <v>7.88</v>
       </c>
       <c r="M59" s="6" t="n">
-        <v>0</v>
+        <v>2.05</v>
       </c>
       <c r="N59" s="5" t="n">
         <v>1</v>
@@ -2834,100 +2840,98 @@
     </row>
     <row r="60" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B60" s="3" t="s"/>
       <c r="C60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F60" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H60" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I60" s="6" t="n">
-        <v>1.19</v>
+        <v>42.58</v>
       </c>
       <c r="J60" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="5" t="n">
-        <v>5.04</v>
+        <v>7.89</v>
       </c>
       <c r="L60" s="5" t="n">
-        <v>5.04</v>
+        <v>7.89</v>
       </c>
       <c r="M60" s="6" t="n">
-        <v>0.06</v>
+        <v>3.36</v>
       </c>
       <c r="N60" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B61" s="3" t="s"/>
       <c r="C61" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F61" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H61" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I61" s="6" t="n">
-        <v>10.99</v>
+        <v>2182.39</v>
       </c>
       <c r="J61" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="5" t="n">
-        <v>7.37</v>
+        <v>7.9</v>
       </c>
       <c r="L61" s="5" t="n">
-        <v>7.37</v>
+        <v>7.9</v>
       </c>
       <c r="M61" s="6" t="n">
-        <v>0.81</v>
+        <v>172.41</v>
       </c>
       <c r="N61" s="5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B62" s="3" t="s"/>
       <c r="C62" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>46</v>
@@ -2942,61 +2946,61 @@
         <v>0</v>
       </c>
       <c r="I62" s="6" t="n">
-        <v>9.99</v>
+        <v>75.74</v>
       </c>
       <c r="J62" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K62" s="5" t="n">
-        <v>6.81</v>
+        <v>7.91</v>
       </c>
       <c r="L62" s="5" t="n">
-        <v>6.81</v>
+        <v>7.91</v>
       </c>
       <c r="M62" s="6" t="n">
-        <v>0.68</v>
+        <v>5.99</v>
       </c>
       <c r="N62" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B63" s="3" t="s"/>
       <c r="C63" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F63" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="H63" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I63" s="6" t="n">
-        <v>7.76</v>
+        <v>19.56</v>
       </c>
       <c r="J63" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K63" s="5" t="n">
-        <v>5.93</v>
+        <v>7.92</v>
       </c>
       <c r="L63" s="5" t="n">
-        <v>5.93</v>
+        <v>7.92</v>
       </c>
       <c r="M63" s="6" t="n">
-        <v>0.46</v>
+        <v>1.55</v>
       </c>
       <c r="N63" s="5" t="n">
         <v>1</v>
@@ -3004,43 +3008,41 @@
     </row>
     <row r="64" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B64" s="3" t="s"/>
       <c r="C64" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F64" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="H64" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I64" s="6" t="n">
-        <v>40.42</v>
+        <v>1</v>
       </c>
       <c r="J64" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K64" s="5" t="n">
-        <v>6.01</v>
+        <v>8</v>
       </c>
       <c r="L64" s="5" t="n">
-        <v>6.01</v>
+        <v>8</v>
       </c>
       <c r="M64" s="6" t="n">
-        <v>2.43</v>
+        <v>0.08</v>
       </c>
       <c r="N64" s="5" t="n">
         <v>1</v>
@@ -3048,43 +3050,41 @@
     </row>
     <row r="65" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B65" s="3" t="s"/>
       <c r="C65" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F65" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H65" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I65" s="6" t="n">
-        <v>28.92</v>
+        <v>2.49</v>
       </c>
       <c r="J65" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K65" s="5" t="n">
-        <v>7.4</v>
+        <v>8.03</v>
       </c>
       <c r="L65" s="5" t="n">
-        <v>7.4</v>
+        <v>8.03</v>
       </c>
       <c r="M65" s="6" t="n">
-        <v>2.14</v>
+        <v>0.2</v>
       </c>
       <c r="N65" s="5" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Criado novo teste em [https://intranet-hom.conciliadora.com.br]
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação de Taxas.xlsx
+++ b/cypress/downloads/Conciliação de Taxas.xlsx
@@ -59,94 +59,94 @@
     <t>Qtde.</t>
   </si>
   <si>
+    <t>000000080683215</t>
+  </si>
+  <si>
+    <t>000000012784869</t>
+  </si>
+  <si>
+    <t>82123891000138</t>
+  </si>
+  <si>
+    <t>EMPRESA MODELO</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>Ticket Flex</t>
+  </si>
+  <si>
+    <t>000000080683312</t>
+  </si>
+  <si>
+    <t>000000008784337</t>
+  </si>
+  <si>
+    <t>TICKET ALIMENTACAO</t>
+  </si>
+  <si>
+    <t>033090890000129</t>
+  </si>
+  <si>
+    <t>Sodexo</t>
+  </si>
+  <si>
+    <t>SODEXO REFEICAO</t>
+  </si>
+  <si>
+    <t>Comprocard</t>
+  </si>
+  <si>
+    <t>Comprocard Crédito</t>
+  </si>
+  <si>
+    <t>000000008784329</t>
+  </si>
+  <si>
+    <t>TICKET REFEICAO</t>
+  </si>
+  <si>
+    <t>000000007815071</t>
+  </si>
+  <si>
+    <t>000000007815066</t>
+  </si>
+  <si>
+    <t>UpBrasil</t>
+  </si>
+  <si>
+    <t>UpBrasil Convênio</t>
+  </si>
+  <si>
+    <t>000000008781052</t>
+  </si>
+  <si>
+    <t>000000008781044</t>
+  </si>
+  <si>
+    <t>033091040000145</t>
+  </si>
+  <si>
+    <t>Cabal</t>
+  </si>
+  <si>
+    <t>CABAL VOUCHER</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>VR REFEICAO</t>
+  </si>
+  <si>
     <t>013998257000126</t>
   </si>
   <si>
-    <t>82123891000138</t>
-  </si>
-  <si>
-    <t>EMPRESA MODELO</t>
-  </si>
-  <si>
     <t>Valecard</t>
   </si>
   <si>
     <t>Valecard Voucher</t>
-  </si>
-  <si>
-    <t>033091040000145</t>
-  </si>
-  <si>
-    <t>VR</t>
-  </si>
-  <si>
-    <t>VR REFEICAO</t>
-  </si>
-  <si>
-    <t>Sodexo</t>
-  </si>
-  <si>
-    <t>SODEXO REFEICAO</t>
-  </si>
-  <si>
-    <t>033090890000129</t>
-  </si>
-  <si>
-    <t>000000080683312</t>
-  </si>
-  <si>
-    <t>000000008784337</t>
-  </si>
-  <si>
-    <t>Ticket</t>
-  </si>
-  <si>
-    <t>TICKET ALIMENTACAO</t>
-  </si>
-  <si>
-    <t>000000008784329</t>
-  </si>
-  <si>
-    <t>TICKET REFEICAO</t>
-  </si>
-  <si>
-    <t>000000080683215</t>
-  </si>
-  <si>
-    <t>000000008781044</t>
-  </si>
-  <si>
-    <t>000000008781052</t>
-  </si>
-  <si>
-    <t>Cabal</t>
-  </si>
-  <si>
-    <t>CABAL VOUCHER</t>
-  </si>
-  <si>
-    <t>000000007815066</t>
-  </si>
-  <si>
-    <t>UpBrasil</t>
-  </si>
-  <si>
-    <t>UpBrasil Convênio</t>
-  </si>
-  <si>
-    <t>000000007815071</t>
-  </si>
-  <si>
-    <t>000000012784869</t>
-  </si>
-  <si>
-    <t>Ticket Flex</t>
-  </si>
-  <si>
-    <t>Comprocard</t>
-  </si>
-  <si>
-    <t>Comprocard Crédito</t>
   </si>
   <si>
     <t>000000001438301</t>
@@ -263,7 +263,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col width="20.57" min="1" max="1" customWidth="1"/>
-    <col width="17.86" min="2" max="2" customWidth="1"/>
+    <col width="18" min="2" max="2" customWidth="1"/>
     <col width="15.43" min="3" max="3" customWidth="1"/>
     <col width="17.71" min="4" max="4" customWidth="1"/>
     <col width="16" min="5" max="5" customWidth="1"/>
@@ -326,39 +326,41 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s"/>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>3.71</v>
+        <v>6.57</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>2.7</v>
+        <v>5.94</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>0.3</v>
+        <v>5.94</v>
       </c>
       <c r="M2" s="6" t="n">
-        <v>0.01</v>
+        <v>0.39</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>1</v>
@@ -366,41 +368,43 @@
     </row>
     <row r="3" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>9.99</v>
+        <v>29.75</v>
       </c>
       <c r="J3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>6.81</v>
+        <v>5.98</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>6.81</v>
+        <v>5.98</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>0.68</v>
+        <v>1.78</v>
       </c>
       <c r="N3" s="5" t="n">
         <v>1</v>
@@ -408,41 +412,43 @@
     </row>
     <row r="4" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>282</v>
+        <v>15.52</v>
       </c>
       <c r="J4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>6.85</v>
+        <v>6.89</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>6.85</v>
+        <v>6.89</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>19.32</v>
+        <v>1.07</v>
       </c>
       <c r="N4" s="5" t="n">
         <v>1</v>
@@ -450,43 +456,41 @@
     </row>
     <row r="5" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s"/>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>0.01</v>
+        <v>4.79</v>
       </c>
       <c r="J5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>0</v>
+        <v>5.85</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>0</v>
+        <v>5.85</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="N5" s="5" t="n">
         <v>1</v>
@@ -494,43 +498,43 @@
     </row>
     <row r="6" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="H6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v>69.44</v>
+        <v>5.79</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>6.9</v>
+        <v>6.04</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>6.9</v>
+        <v>6.04</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>4.79</v>
+        <v>0.35</v>
       </c>
       <c r="N6" s="5" t="n">
         <v>1</v>
@@ -538,43 +542,43 @@
     </row>
     <row r="7" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v>15.52</v>
+        <v>150</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>6.89</v>
+        <v>6</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>6.89</v>
+        <v>6</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>1.07</v>
+        <v>9</v>
       </c>
       <c r="N7" s="5" t="n">
         <v>1</v>
@@ -582,43 +586,43 @@
     </row>
     <row r="8" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>6.22</v>
+        <v>31.95</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>5.95</v>
+        <v>5.01</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>5.95</v>
+        <v>5.01</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>0.37</v>
+        <v>1.6</v>
       </c>
       <c r="N8" s="5" t="n">
         <v>1</v>
@@ -626,43 +630,41 @@
     </row>
     <row r="9" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s"/>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="H9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>29.75</v>
+        <v>9.59</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>5.98</v>
+        <v>5.94</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>5.98</v>
+        <v>5.94</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>1.78</v>
+        <v>0.57</v>
       </c>
       <c r="N9" s="5" t="n">
         <v>1</v>
@@ -670,43 +672,41 @@
     </row>
     <row r="10" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s"/>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="H10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>5.79</v>
+        <v>12.71</v>
       </c>
       <c r="J10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>6.04</v>
+        <v>5.9</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>6.04</v>
+        <v>5.9</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>1</v>
@@ -714,43 +714,41 @@
     </row>
     <row r="11" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s"/>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="H11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="6" t="n">
-        <v>0.99</v>
+        <v>25.47</v>
       </c>
       <c r="J11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>6.06</v>
+        <v>5.89</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>6.06</v>
+        <v>5.89</v>
       </c>
       <c r="M11" s="6" t="n">
-        <v>0.06</v>
+        <v>1.5</v>
       </c>
       <c r="N11" s="5" t="n">
         <v>1</v>
@@ -758,43 +756,43 @@
     </row>
     <row r="12" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="H12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="6" t="n">
-        <v>150</v>
+        <v>6.08</v>
       </c>
       <c r="J12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>6</v>
+        <v>5.92</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>6</v>
+        <v>5.92</v>
       </c>
       <c r="M12" s="6" t="n">
-        <v>9</v>
+        <v>0.36</v>
       </c>
       <c r="N12" s="5" t="n">
         <v>1</v>
@@ -802,43 +800,43 @@
     </row>
     <row r="13" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="6" t="n">
-        <v>40.42</v>
+        <v>20.25</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>6.01</v>
+        <v>5.98</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>6.01</v>
+        <v>5.98</v>
       </c>
       <c r="M13" s="6" t="n">
-        <v>2.43</v>
+        <v>1.21</v>
       </c>
       <c r="N13" s="5" t="n">
         <v>1</v>
@@ -846,25 +844,25 @@
     </row>
     <row r="14" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>0</v>
@@ -890,43 +888,41 @@
     </row>
     <row r="15" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s"/>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="H15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="6" t="n">
-        <v>6.08</v>
+        <v>2.49</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>5.92</v>
+        <v>8.03</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>5.92</v>
+        <v>8.03</v>
       </c>
       <c r="M15" s="6" t="n">
-        <v>0.36</v>
+        <v>0.2</v>
       </c>
       <c r="N15" s="5" t="n">
         <v>1</v>
@@ -934,41 +930,41 @@
     </row>
     <row r="16" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s"/>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="6" t="n">
-        <v>4.98</v>
+        <v>39.65</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="5" t="n">
-        <v>5.02</v>
+        <v>6.51</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>5.02</v>
+        <v>6.51</v>
       </c>
       <c r="M16" s="6" t="n">
-        <v>0.25</v>
+        <v>2.58</v>
       </c>
       <c r="N16" s="5" t="n">
         <v>1</v>
@@ -976,41 +972,41 @@
     </row>
     <row r="17" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s"/>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="6" t="n">
-        <v>1.19</v>
+        <v>4.98</v>
       </c>
       <c r="J17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>5.04</v>
+        <v>5.02</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>5.04</v>
+        <v>5.02</v>
       </c>
       <c r="M17" s="6" t="n">
-        <v>0.06</v>
+        <v>0.25</v>
       </c>
       <c r="N17" s="5" t="n">
         <v>1</v>
@@ -1018,41 +1014,41 @@
     </row>
     <row r="18" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s"/>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="6" t="n">
-        <v>31.15</v>
+        <v>33</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>6.48</v>
+        <v>5.91</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>6.48</v>
+        <v>5.91</v>
       </c>
       <c r="M18" s="6" t="n">
-        <v>2.02</v>
+        <v>1.95</v>
       </c>
       <c r="N18" s="5" t="n">
         <v>1</v>
@@ -1060,41 +1056,43 @@
     </row>
     <row r="19" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3" t="s"/>
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="6" t="n">
-        <v>82.34</v>
+        <v>22.1</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>6.5</v>
+        <v>5.02</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>6.5</v>
+        <v>5.02</v>
       </c>
       <c r="M19" s="6" t="n">
-        <v>5.35</v>
+        <v>1.11</v>
       </c>
       <c r="N19" s="5" t="n">
         <v>1</v>
@@ -1102,41 +1100,41 @@
     </row>
     <row r="20" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s"/>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="6" t="n">
-        <v>39.65</v>
+        <v>19.56</v>
       </c>
       <c r="J20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>6.51</v>
+        <v>7.92</v>
       </c>
       <c r="L20" s="5" t="n">
-        <v>6.51</v>
+        <v>7.92</v>
       </c>
       <c r="M20" s="6" t="n">
-        <v>2.58</v>
+        <v>1.55</v>
       </c>
       <c r="N20" s="5" t="n">
         <v>1</v>
@@ -1144,16 +1142,14 @@
     </row>
     <row r="21" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s"/>
       <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>37</v>
@@ -1168,19 +1164,19 @@
         <v>0</v>
       </c>
       <c r="I21" s="6" t="n">
-        <v>10.99</v>
+        <v>31.15</v>
       </c>
       <c r="J21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>7.37</v>
+        <v>6.48</v>
       </c>
       <c r="L21" s="5" t="n">
-        <v>7.37</v>
+        <v>6.48</v>
       </c>
       <c r="M21" s="6" t="n">
-        <v>0.81</v>
+        <v>2.02</v>
       </c>
       <c r="N21" s="5" t="n">
         <v>1</v>
@@ -1190,41 +1186,39 @@
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="B22" s="3" t="s"/>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F22" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="6" t="n">
-        <v>28.92</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>7.4</v>
+        <v>8</v>
       </c>
       <c r="L22" s="5" t="n">
-        <v>7.4</v>
+        <v>8</v>
       </c>
       <c r="M22" s="6" t="n">
-        <v>2.14</v>
+        <v>0.08</v>
       </c>
       <c r="N22" s="5" t="n">
         <v>1</v>
@@ -1232,43 +1226,41 @@
     </row>
     <row r="23" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s"/>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F23" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="6" t="n">
-        <v>42.24</v>
+        <v>282</v>
       </c>
       <c r="J23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>5</v>
+        <v>6.85</v>
       </c>
       <c r="L23" s="5" t="n">
-        <v>5</v>
+        <v>6.85</v>
       </c>
       <c r="M23" s="6" t="n">
-        <v>2.11</v>
+        <v>19.32</v>
       </c>
       <c r="N23" s="5" t="n">
         <v>1</v>
@@ -1276,43 +1268,43 @@
     </row>
     <row r="24" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="6" t="n">
-        <v>31.95</v>
+        <v>42.24</v>
       </c>
       <c r="J24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K24" s="5" t="n">
-        <v>5.01</v>
+        <v>5</v>
       </c>
       <c r="L24" s="5" t="n">
-        <v>5.01</v>
+        <v>5</v>
       </c>
       <c r="M24" s="6" t="n">
-        <v>1.6</v>
+        <v>2.11</v>
       </c>
       <c r="N24" s="5" t="n">
         <v>1</v>
@@ -1320,16 +1312,14 @@
     </row>
     <row r="25" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s"/>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>37</v>
@@ -1344,19 +1334,19 @@
         <v>0</v>
       </c>
       <c r="I25" s="6" t="n">
-        <v>22.1</v>
+        <v>82.34</v>
       </c>
       <c r="J25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K25" s="5" t="n">
-        <v>5.02</v>
+        <v>6.5</v>
       </c>
       <c r="L25" s="5" t="n">
-        <v>5.02</v>
+        <v>6.5</v>
       </c>
       <c r="M25" s="6" t="n">
-        <v>1.11</v>
+        <v>5.35</v>
       </c>
       <c r="N25" s="5" t="n">
         <v>1</v>
@@ -1364,43 +1354,43 @@
     </row>
     <row r="26" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="6" t="n">
-        <v>6.57</v>
+        <v>6.22</v>
       </c>
       <c r="J26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K26" s="5" t="n">
-        <v>5.94</v>
+        <v>5.95</v>
       </c>
       <c r="L26" s="5" t="n">
-        <v>5.94</v>
+        <v>5.95</v>
       </c>
       <c r="M26" s="6" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="N26" s="5" t="n">
         <v>1</v>
@@ -1408,43 +1398,43 @@
     </row>
     <row r="27" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="6" t="n">
-        <v>20.25</v>
+        <v>0.99</v>
       </c>
       <c r="J27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K27" s="5" t="n">
-        <v>5.98</v>
+        <v>6.06</v>
       </c>
       <c r="L27" s="5" t="n">
-        <v>5.98</v>
+        <v>6.06</v>
       </c>
       <c r="M27" s="6" t="n">
-        <v>1.21</v>
+        <v>0.06</v>
       </c>
       <c r="N27" s="5" t="n">
         <v>1</v>
@@ -1452,14 +1442,14 @@
     </row>
     <row r="28" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s"/>
       <c r="C28" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>42</v>
@@ -1474,19 +1464,19 @@
         <v>0</v>
       </c>
       <c r="I28" s="6" t="n">
-        <v>4.79</v>
+        <v>3.71</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K28" s="5" t="n">
-        <v>5.85</v>
+        <v>2.7</v>
       </c>
       <c r="L28" s="5" t="n">
-        <v>5.85</v>
+        <v>0.3</v>
       </c>
       <c r="M28" s="6" t="n">
-        <v>0.28</v>
+        <v>0.01</v>
       </c>
       <c r="N28" s="5" t="n">
         <v>1</v>
@@ -1494,41 +1484,43 @@
     </row>
     <row r="29" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="3" t="s"/>
-      <c r="C29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F29" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="6" t="n">
-        <v>25.47</v>
+        <v>69.44</v>
       </c>
       <c r="J29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="5" t="n">
-        <v>5.89</v>
+        <v>6.9</v>
       </c>
       <c r="L29" s="5" t="n">
-        <v>5.89</v>
+        <v>6.9</v>
       </c>
       <c r="M29" s="6" t="n">
-        <v>1.5</v>
+        <v>4.79</v>
       </c>
       <c r="N29" s="5" t="n">
         <v>1</v>
@@ -1536,41 +1528,41 @@
     </row>
     <row r="30" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s"/>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="6" t="n">
-        <v>12.71</v>
+        <v>26</v>
       </c>
       <c r="J30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K30" s="5" t="n">
-        <v>5.9</v>
+        <v>7.88</v>
       </c>
       <c r="L30" s="5" t="n">
-        <v>5.9</v>
+        <v>7.88</v>
       </c>
       <c r="M30" s="6" t="n">
-        <v>0.75</v>
+        <v>2.05</v>
       </c>
       <c r="N30" s="5" t="n">
         <v>1</v>
@@ -1578,41 +1570,43 @@
     </row>
     <row r="31" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="3" t="s"/>
-      <c r="C31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F31" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="6" t="n">
-        <v>33</v>
+        <v>0.01</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K31" s="5" t="n">
-        <v>5.91</v>
+        <v>0</v>
       </c>
       <c r="L31" s="5" t="n">
-        <v>5.91</v>
+        <v>0</v>
       </c>
       <c r="M31" s="6" t="n">
-        <v>1.95</v>
+        <v>0</v>
       </c>
       <c r="N31" s="5" t="n">
         <v>1</v>
@@ -1620,41 +1614,41 @@
     </row>
     <row r="32" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="3" t="s"/>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="6" t="n">
-        <v>7.76</v>
+        <v>1.19</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="5" t="n">
-        <v>5.93</v>
+        <v>5.04</v>
       </c>
       <c r="L32" s="5" t="n">
-        <v>5.93</v>
+        <v>5.04</v>
       </c>
       <c r="M32" s="6" t="n">
-        <v>0.46</v>
+        <v>0.06</v>
       </c>
       <c r="N32" s="5" t="n">
         <v>1</v>
@@ -1662,41 +1656,43 @@
     </row>
     <row r="33" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I33" s="6" t="n">
-        <v>9.59</v>
+        <v>10.99</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="5" t="n">
-        <v>5.94</v>
+        <v>7.37</v>
       </c>
       <c r="L33" s="5" t="n">
-        <v>5.94</v>
+        <v>7.37</v>
       </c>
       <c r="M33" s="6" t="n">
-        <v>0.57</v>
+        <v>0.81</v>
       </c>
       <c r="N33" s="5" t="n">
         <v>1</v>
@@ -1704,41 +1700,41 @@
     </row>
     <row r="34" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s"/>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="n">
-        <v>26</v>
+        <v>9.99</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="5" t="n">
-        <v>7.88</v>
+        <v>6.81</v>
       </c>
       <c r="L34" s="5" t="n">
-        <v>7.88</v>
+        <v>6.81</v>
       </c>
       <c r="M34" s="6" t="n">
-        <v>2.05</v>
+        <v>0.68</v>
       </c>
       <c r="N34" s="5" t="n">
         <v>1</v>
@@ -1746,41 +1742,41 @@
     </row>
     <row r="35" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s"/>
       <c r="C35" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="n">
-        <v>19.56</v>
+        <v>7.76</v>
       </c>
       <c r="J35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K35" s="5" t="n">
-        <v>7.92</v>
+        <v>5.93</v>
       </c>
       <c r="L35" s="5" t="n">
-        <v>7.92</v>
+        <v>5.93</v>
       </c>
       <c r="M35" s="6" t="n">
-        <v>1.55</v>
+        <v>0.46</v>
       </c>
       <c r="N35" s="5" t="n">
         <v>1</v>
@@ -1788,41 +1784,43 @@
     </row>
     <row r="36" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="3" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I36" s="6" t="n">
-        <v>1</v>
+        <v>40.42</v>
       </c>
       <c r="J36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K36" s="5" t="n">
-        <v>8</v>
+        <v>6.01</v>
       </c>
       <c r="L36" s="5" t="n">
-        <v>8</v>
+        <v>6.01</v>
       </c>
       <c r="M36" s="6" t="n">
-        <v>0.08</v>
+        <v>2.43</v>
       </c>
       <c r="N36" s="5" t="n">
         <v>1</v>
@@ -1830,41 +1828,43 @@
     </row>
     <row r="37" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="3" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C37" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F37" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I37" s="6" t="n">
-        <v>2.49</v>
+        <v>28.92</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K37" s="5" t="n">
-        <v>8.03</v>
+        <v>7.4</v>
       </c>
       <c r="L37" s="5" t="n">
-        <v>8.03</v>
+        <v>7.4</v>
       </c>
       <c r="M37" s="6" t="n">
-        <v>0.2</v>
+        <v>2.14</v>
       </c>
       <c r="N37" s="5" t="n">
         <v>1</v>
@@ -1874,39 +1874,41 @@
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="3" t="s"/>
+      <c r="B38" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F38" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I38" s="6" t="n">
-        <v>133.63</v>
+        <v>62.05</v>
       </c>
       <c r="J38" s="5" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="K38" s="5" t="n">
-        <v>2.81</v>
+        <v>6.01</v>
       </c>
       <c r="L38" s="5" t="n">
-        <v>0.41</v>
+        <v>6.01</v>
       </c>
       <c r="M38" s="6" t="n">
-        <v>0.55</v>
+        <v>3.73</v>
       </c>
       <c r="N38" s="5" t="n">
         <v>2</v>
@@ -1914,43 +1916,43 @@
     </row>
     <row r="39" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="H39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I39" s="6" t="n">
-        <v>33.9</v>
+        <v>145.29</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>6.02</v>
+        <v>6.8</v>
       </c>
       <c r="L39" s="5" t="n">
-        <v>6.02</v>
+        <v>6.8</v>
       </c>
       <c r="M39" s="6" t="n">
-        <v>2.04</v>
+        <v>9.88</v>
       </c>
       <c r="N39" s="5" t="n">
         <v>2</v>
@@ -1958,43 +1960,43 @@
     </row>
     <row r="40" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="6" t="n">
-        <v>0.02</v>
+        <v>58.01</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K40" s="5" t="n">
-        <v>0</v>
+        <v>7.38</v>
       </c>
       <c r="L40" s="5" t="n">
-        <v>0</v>
+        <v>7.38</v>
       </c>
       <c r="M40" s="6" t="n">
-        <v>0</v>
+        <v>4.28</v>
       </c>
       <c r="N40" s="5" t="n">
         <v>2</v>
@@ -2002,43 +2004,41 @@
     </row>
     <row r="41" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B41" s="3" t="s"/>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F41" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="H41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="6" t="n">
-        <v>62.05</v>
+        <v>75.74</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>6.01</v>
+        <v>7.91</v>
       </c>
       <c r="L41" s="5" t="n">
-        <v>6.01</v>
+        <v>7.91</v>
       </c>
       <c r="M41" s="6" t="n">
-        <v>3.73</v>
+        <v>5.99</v>
       </c>
       <c r="N41" s="5" t="n">
         <v>2</v>
@@ -2046,43 +2046,41 @@
     </row>
     <row r="42" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s"/>
       <c r="C42" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F42" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
-        <v>73.57</v>
+        <v>133.63</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="K42" s="5" t="n">
-        <v>6.01</v>
+        <v>2.81</v>
       </c>
       <c r="L42" s="5" t="n">
-        <v>6.01</v>
+        <v>0.41</v>
       </c>
       <c r="M42" s="6" t="n">
-        <v>4.42</v>
+        <v>0.55</v>
       </c>
       <c r="N42" s="5" t="n">
         <v>2</v>
@@ -2090,43 +2088,43 @@
     </row>
     <row r="43" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F43" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
-        <v>58.01</v>
+        <v>0.02</v>
       </c>
       <c r="J43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="5" t="n">
-        <v>7.38</v>
+        <v>0</v>
       </c>
       <c r="L43" s="5" t="n">
-        <v>7.38</v>
+        <v>0</v>
       </c>
       <c r="M43" s="6" t="n">
-        <v>4.28</v>
+        <v>0</v>
       </c>
       <c r="N43" s="5" t="n">
         <v>2</v>
@@ -2136,41 +2134,39 @@
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="B44" s="3" t="s"/>
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F44" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
-        <v>68.38</v>
+        <v>42.58</v>
       </c>
       <c r="J44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K44" s="5" t="n">
-        <v>9.07</v>
+        <v>7.89</v>
       </c>
       <c r="L44" s="5" t="n">
-        <v>9.07</v>
+        <v>7.89</v>
       </c>
       <c r="M44" s="6" t="n">
-        <v>6.2</v>
+        <v>3.36</v>
       </c>
       <c r="N44" s="5" t="n">
         <v>2</v>
@@ -2178,43 +2174,43 @@
     </row>
     <row r="45" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F45" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
-        <v>8.46</v>
+        <v>73.57</v>
       </c>
       <c r="J45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="5" t="n">
-        <v>5.91</v>
+        <v>6.01</v>
       </c>
       <c r="L45" s="5" t="n">
-        <v>5.91</v>
+        <v>6.01</v>
       </c>
       <c r="M45" s="6" t="n">
-        <v>0.5</v>
+        <v>4.42</v>
       </c>
       <c r="N45" s="5" t="n">
         <v>2</v>
@@ -2222,43 +2218,43 @@
     </row>
     <row r="46" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F46" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
-        <v>145.29</v>
+        <v>68.38</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K46" s="5" t="n">
-        <v>6.8</v>
+        <v>9.07</v>
       </c>
       <c r="L46" s="5" t="n">
-        <v>6.8</v>
+        <v>9.07</v>
       </c>
       <c r="M46" s="6" t="n">
-        <v>9.88</v>
+        <v>6.2</v>
       </c>
       <c r="N46" s="5" t="n">
         <v>2</v>
@@ -2266,41 +2262,43 @@
     </row>
     <row r="47" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>45170</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="3" t="s"/>
-      <c r="C47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="4" t="n">
-        <v>45170</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="H47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
-        <v>42.58</v>
+        <v>8.46</v>
       </c>
       <c r="J47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K47" s="5" t="n">
-        <v>7.89</v>
+        <v>5.91</v>
       </c>
       <c r="L47" s="5" t="n">
-        <v>7.89</v>
+        <v>5.91</v>
       </c>
       <c r="M47" s="6" t="n">
-        <v>3.36</v>
+        <v>0.5</v>
       </c>
       <c r="N47" s="5" t="n">
         <v>2</v>
@@ -2308,41 +2306,43 @@
     </row>
     <row r="48" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="3" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F48" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
-        <v>75.74</v>
+        <v>33.9</v>
       </c>
       <c r="J48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="5" t="n">
-        <v>7.91</v>
+        <v>6.02</v>
       </c>
       <c r="L48" s="5" t="n">
-        <v>7.91</v>
+        <v>6.02</v>
       </c>
       <c r="M48" s="6" t="n">
-        <v>5.99</v>
+        <v>2.04</v>
       </c>
       <c r="N48" s="5" t="n">
         <v>2</v>
@@ -2350,23 +2350,23 @@
     </row>
     <row r="49" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B49" s="3" t="s"/>
       <c r="C49" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F49" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H49" s="5" t="n">
         <v>0</v>
@@ -2392,43 +2392,43 @@
     </row>
     <row r="50" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F50" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I50" s="6" t="n">
-        <v>121.15</v>
+        <v>490.6</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K50" s="5" t="n">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="L50" s="5" t="n">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="M50" s="6" t="n">
-        <v>7.26</v>
+        <v>29.44</v>
       </c>
       <c r="N50" s="5" t="n">
         <v>3</v>
@@ -2436,43 +2436,43 @@
     </row>
     <row r="51" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F51" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I51" s="6" t="n">
-        <v>490.6</v>
+        <v>37.18</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K51" s="5" t="n">
-        <v>6</v>
+        <v>5.97</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>6</v>
+        <v>5.97</v>
       </c>
       <c r="M51" s="6" t="n">
-        <v>29.44</v>
+        <v>2.22</v>
       </c>
       <c r="N51" s="5" t="n">
         <v>3</v>
@@ -2480,25 +2480,25 @@
     </row>
     <row r="52" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F52" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H52" s="5" t="n">
         <v>0</v>
@@ -2524,43 +2524,43 @@
     </row>
     <row r="53" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F53" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
-        <v>37.18</v>
+        <v>121.15</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K53" s="5" t="n">
-        <v>5.97</v>
+        <v>5.99</v>
       </c>
       <c r="L53" s="5" t="n">
-        <v>5.97</v>
+        <v>5.99</v>
       </c>
       <c r="M53" s="6" t="n">
-        <v>2.22</v>
+        <v>7.26</v>
       </c>
       <c r="N53" s="5" t="n">
         <v>3</v>
@@ -2568,43 +2568,43 @@
     </row>
     <row r="54" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F54" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H54" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I54" s="6" t="n">
-        <v>174.71</v>
+        <v>299.89</v>
       </c>
       <c r="J54" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="5" t="n">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="L54" s="5" t="n">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="M54" s="6" t="n">
-        <v>10.47</v>
+        <v>17.99</v>
       </c>
       <c r="N54" s="5" t="n">
         <v>4</v>
@@ -2612,43 +2612,43 @@
     </row>
     <row r="55" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F55" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I55" s="6" t="n">
-        <v>299.89</v>
+        <v>174.71</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="5" t="n">
-        <v>6</v>
+        <v>5.99</v>
       </c>
       <c r="L55" s="5" t="n">
-        <v>6</v>
+        <v>5.99</v>
       </c>
       <c r="M55" s="6" t="n">
-        <v>17.99</v>
+        <v>10.47</v>
       </c>
       <c r="N55" s="5" t="n">
         <v>4</v>
@@ -2656,25 +2656,25 @@
     </row>
     <row r="56" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H56" s="5" t="n">
         <v>0</v>
@@ -2700,25 +2700,25 @@
     </row>
     <row r="57" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F57" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H57" s="5" t="n">
         <v>0</v>
@@ -2744,43 +2744,43 @@
     </row>
     <row r="58" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F58" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I58" s="6" t="n">
-        <v>104.65</v>
+        <v>40.29</v>
       </c>
       <c r="J58" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K58" s="5" t="n">
-        <v>6.01</v>
+        <v>6.03</v>
       </c>
       <c r="L58" s="5" t="n">
-        <v>6.01</v>
+        <v>6.03</v>
       </c>
       <c r="M58" s="6" t="n">
-        <v>6.29</v>
+        <v>2.43</v>
       </c>
       <c r="N58" s="5" t="n">
         <v>5</v>
@@ -2788,43 +2788,43 @@
     </row>
     <row r="59" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F59" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H59" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I59" s="6" t="n">
-        <v>40.29</v>
+        <v>104.65</v>
       </c>
       <c r="J59" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="5" t="n">
-        <v>6.03</v>
+        <v>6.01</v>
       </c>
       <c r="L59" s="5" t="n">
-        <v>6.03</v>
+        <v>6.01</v>
       </c>
       <c r="M59" s="6" t="n">
-        <v>2.43</v>
+        <v>6.29</v>
       </c>
       <c r="N59" s="5" t="n">
         <v>5</v>
@@ -2832,25 +2832,25 @@
     </row>
     <row r="60" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F60" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H60" s="5" t="n">
         <v>0</v>
@@ -2876,25 +2876,25 @@
     </row>
     <row r="61" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F61" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H61" s="5" t="n">
         <v>0</v>
@@ -2920,23 +2920,23 @@
     </row>
     <row r="62" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s"/>
       <c r="C62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F62" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H62" s="5" t="n">
         <v>0</v>
@@ -2962,25 +2962,25 @@
     </row>
     <row r="63" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F63" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H63" s="5" t="n">
         <v>0</v>
@@ -3006,25 +3006,25 @@
     </row>
     <row r="64" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F64" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H64" s="5" t="n">
         <v>0</v>
@@ -3050,23 +3050,23 @@
     </row>
     <row r="65" spans="1:14" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B65" s="3" t="s"/>
       <c r="C65" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F65" s="4" t="n">
         <v>45170</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H65" s="5" t="n">
         <v>0</v>

</xml_diff>